<commit_message>
funcionan perfectamente las funciones de dano, se aplicaron danos a dos elementos y funciona bien. Esto fue aplicado a un marco de un nivel con elementos diagonales
</commit_message>
<xml_diff>
--- a/pruebas_excel/ETABS_modelo/ETABS/revision_3_marco_con_dano/datos_prueba3.xlsx
+++ b/pruebas_excel/ETABS_modelo/ETABS/revision_3_marco_con_dano/datos_prueba3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral_error\pruebas_excel\ETABS_modelo\ETABS\revision_3_marco_con_dano\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\ETABS_modelo\ETABS\revision_3_marco_con_dano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C3F7126-8017-40F7-BE53-B2A4F9EABA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF459FE4-60AC-4485-96CA-7AFE510D24BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="3315" windowWidth="12000" windowHeight="7995" firstSheet="30" activeTab="30" xr2:uid="{7D1F8C59-414A-4CDF-9139-FB7D48E715A8}"/>
+    <workbookView xWindow="12405" yWindow="4230" windowWidth="12000" windowHeight="7995" firstSheet="30" activeTab="30" xr2:uid="{1108F7E5-EE7C-4239-A8C2-AFF9DC0EF2BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Assembled Joint Masses" sheetId="1" r:id="rId1"/>
@@ -1410,7 +1410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E2C442-AD7F-4712-9D9C-56CC31CB11D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE83F56-A8EF-4DBF-AA85-3D93CBDCAA12}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1827,7 +1827,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF922A87-BBAE-4F1D-B6A9-7F119374206F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9478548B-5118-4356-90D8-101DC853F820}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2224,7 +2224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55873B82-4663-4295-9D48-085898835CD8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BE5B0D-6A2F-4A93-AC2C-50B71F113FCE}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2624,7 +2624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2893B0-5C67-4BDF-83EA-BC62DEFC1639}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2A7381-3CB4-48A5-96AD-E4A8217F5D90}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2979,7 +2979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B2CEF5-6D27-4018-891D-53BA8DE0C5D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6870AD5D-AEF1-4457-9E7A-00B4863954B0}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3253,7 +3253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E06F2BA-CA19-4B2E-9E7F-9A11C63FDF3D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FDB89A-9348-4228-AEF6-AF9930E7A2C6}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3565,10 +3565,10 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E709369E-FA33-4B34-BD96-FFF9B86FF8AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B843E9-DFE4-4AE3-B02B-084AA51A807F}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C15"/>
     </sheetView>
   </sheetViews>
@@ -3971,7 +3971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9491485C-A38A-446F-B8F7-A569DB8D30DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B150B06-4D33-48F5-BB4A-8FEAF4558352}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4283,7 +4283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BDB6E2-6345-49A8-BCE5-BEA8E4AFF74A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7146EA3-9722-4D3A-87DD-0D75BDEE2D63}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4464,7 +4464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC723964-3298-4DCF-9CDA-B460E581F4E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0C103D-B759-4E28-BDC3-8DD0DC5CCEF2}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4790,7 +4790,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C11906A-C985-4B8B-BE44-F3BE6088C67F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3506CFEF-254F-44A5-9A4A-B5EDCBEEFEFA}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4882,7 +4882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3C5642-287D-43A7-BACA-CEF413DBF03C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83221338-8DD4-4A4B-A77E-35179DC72205}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4995,7 +4995,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09ED0EBF-8A40-4912-AB3C-B637D589825F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E391ABD-C050-4DD7-85ED-90F56AB50024}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5202,7 +5202,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D1F587-1C6B-45BB-A17E-55745A7A05C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590C13C5-2A7E-43A0-A875-42F37BE79724}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5390,7 +5390,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD5B54B-0113-4848-9965-3899CB8B0D78}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5306E668-4674-48CE-88FC-2201D88114D6}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5676,7 +5676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE669B01-6F0D-4F31-BD53-34558535B83C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B1EA7F-86D3-4E0C-8E80-CBF2499622F9}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5813,7 +5813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED79363-C608-4E3C-8716-CA32E7118605}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A5C4F1-BA9A-4F35-B467-89BB4A6D10CA}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5990,7 +5990,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE7BA9B-4EA0-4E1F-949B-D391FE2E7D3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1E099B-E980-4271-8A62-F5596DD9857D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6039,11 +6039,11 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4626EF32-0392-419D-8D36-676AAF4EE672}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F9E0A0-B189-4EFF-8ECB-01F3CCEFA662}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A7"/>
+      <selection activeCell="A4" sqref="A4:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6190,7 +6190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2229B2-3216-4A82-B426-F8C5C2416CD9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674515EC-FABD-44DF-9E7E-401FD958ACDA}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6516,7 +6516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78613BB7-6B9D-4169-BAAB-7D276345DADA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D6A5AB-B42B-42EF-B904-9016BE2983FF}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6576,7 +6576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176EEE3D-0136-45A1-BEEB-4244C09999A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2863531-406A-430E-87BD-D1A88C822BCB}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6680,7 +6680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A720EE4-8AFB-43CB-AD53-700F66397FF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3B6526-088B-4E1B-BB31-CC71C20E6CFA}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6853,7 +6853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5D2FEB-CC9B-4408-8ED5-6B86EF2D33FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8C7A18-925F-4EB6-9D23-680231FB1C42}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6953,7 +6953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C8B161-02B6-42EA-9E39-F76F891B1ED6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232BD04B-EAE9-48EC-80A3-7030A9BE29D4}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -7112,7 +7112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936102CE-EC0D-422D-B65D-1C910BE55C6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60F2443-A839-473C-8EC1-2308F09D0501}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7245,7 +7245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B94A93-D243-4B15-A9B5-B1314FD1EE56}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AE323D-8169-4A3A-B5B6-B72036F5584B}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7418,11 +7418,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4674D61D-7847-495C-8160-9F80D9095A44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E58660-77AF-4DEB-AC51-8EB56E7E1162}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C8"/>
+      <selection activeCell="B4" sqref="B4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7551,7 +7551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF99E58A-CACB-4252-8B89-71AB70BA332F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2541EC49-4831-4E5C-B5F1-7E31C4D084CA}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7724,7 +7724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6406C11-8A34-4FB1-9C38-A7F4E02A069F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F8903F-5C46-461B-9208-57025B7FD9B8}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7784,7 +7784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D79405-CBA4-4EC7-81D3-6447D1F28FE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C0B1E2-CF61-4D62-BF2B-E389D0E6B00F}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
el AG ya esta devolviendo resultados correctos en el marco de un nivel
</commit_message>
<xml_diff>
--- a/pruebas_excel/ETABS_modelo/ETABS/revision_3_marco_con_dano/datos_prueba3.xlsx
+++ b/pruebas_excel/ETABS_modelo/ETABS/revision_3_marco_con_dano/datos_prueba3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\ETABS_modelo\ETABS\revision_3_marco_con_dano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF459FE4-60AC-4485-96CA-7AFE510D24BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF99E7A5-CEFE-4493-8EDF-1358E6DC7FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12405" yWindow="4230" windowWidth="12000" windowHeight="7995" firstSheet="30" activeTab="30" xr2:uid="{1108F7E5-EE7C-4239-A8C2-AFF9DC0EF2BC}"/>
+    <workbookView xWindow="-30" yWindow="5115" windowWidth="12000" windowHeight="7995" firstSheet="30" activeTab="30" xr2:uid="{DFBB41F5-BB15-4BFD-B3A1-9CBA1652E7F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Assembled Joint Masses" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="289">
   <si>
     <t>TABLE:  Assembled Joint Masses</t>
   </si>
@@ -197,103 +197,79 @@
     <t>IEndStory</t>
   </si>
   <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Below</t>
+  </si>
+  <si>
+    <t>cb24113d-54f5-4e59-9b3d-c7c989424acb</t>
+  </si>
+  <si>
+    <t>TABLE:  Brace Object Connectivity</t>
+  </si>
+  <si>
+    <t>BraceBay</t>
+  </si>
+  <si>
+    <t>787cb99f-13a1-4917-8c24-4948dae85db4</t>
+  </si>
+  <si>
+    <t>TABLE:  Column Bays</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>5fcc99e6-3cf7-451f-9a60-18050e8771c9</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>191d4109-5899-43d2-a5ff-53c5a9dfd341</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>b0cfb463-b38a-4aa0-8243-e34d97cd653d</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>ea17836c-b6b3-4963-8acd-2a89999fdac3</t>
+  </si>
+  <si>
+    <t>TABLE:  Column Object Connectivity</t>
+  </si>
+  <si>
+    <t>ColumnBay</t>
+  </si>
+  <si>
+    <t>4f1dddaf-eecb-41ed-bb8b-930f6bfca92f</t>
+  </si>
+  <si>
+    <t>b89ac87a-c3ac-48c6-a32d-dc133d780ba9</t>
+  </si>
+  <si>
+    <t>c2a10de6-2bc0-40a1-b5a1-b3508b1f592e</t>
+  </si>
+  <si>
+    <t>26c8d49e-95c3-4c94-89c6-4901faa9855d</t>
+  </si>
+  <si>
+    <t>TABLE:  Diaphragm Definitions</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Rigidity Type</t>
+  </si>
+  <si>
     <t>D1</t>
-  </si>
-  <si>
-    <t>Below</t>
-  </si>
-  <si>
-    <t>500dd9c8-1d93-4588-884c-fd10bcfa88e1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>bb870a0f-e673-429e-8f21-ae5f4d126a7c</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>ab1b5781-d07e-458c-990d-1ccc5e4cdb86</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>cb24113d-54f5-4e59-9b3d-c7c989424acb</t>
-  </si>
-  <si>
-    <t>TABLE:  Brace Object Connectivity</t>
-  </si>
-  <si>
-    <t>BraceBay</t>
-  </si>
-  <si>
-    <t>6b88ea5e-f567-4dd8-81fb-bf5d53de9233</t>
-  </si>
-  <si>
-    <t>e3e5969b-6194-46a7-a4c0-2ba1a2709832</t>
-  </si>
-  <si>
-    <t>f189a129-3b44-4b61-a397-47e79ed1421c</t>
-  </si>
-  <si>
-    <t>787cb99f-13a1-4917-8c24-4948dae85db4</t>
-  </si>
-  <si>
-    <t>TABLE:  Column Bays</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>5fcc99e6-3cf7-451f-9a60-18050e8771c9</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>191d4109-5899-43d2-a5ff-53c5a9dfd341</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>b0cfb463-b38a-4aa0-8243-e34d97cd653d</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>ea17836c-b6b3-4963-8acd-2a89999fdac3</t>
-  </si>
-  <si>
-    <t>TABLE:  Column Object Connectivity</t>
-  </si>
-  <si>
-    <t>ColumnBay</t>
-  </si>
-  <si>
-    <t>4f1dddaf-eecb-41ed-bb8b-930f6bfca92f</t>
-  </si>
-  <si>
-    <t>b89ac87a-c3ac-48c6-a32d-dc133d780ba9</t>
-  </si>
-  <si>
-    <t>c2a10de6-2bc0-40a1-b5a1-b3508b1f592e</t>
-  </si>
-  <si>
-    <t>26c8d49e-95c3-4c94-89c6-4901faa9855d</t>
-  </si>
-  <si>
-    <t>TABLE:  Diaphragm Definitions</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Rigidity Type</t>
   </si>
   <si>
     <t>Rigid</t>
@@ -1410,7 +1386,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE83F56-A8EF-4DBF-AA85-3D93CBDCAA12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE6C8B8-C9CA-49D2-AB5B-5D98168C69CE}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1528,13 +1504,13 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1.0337000000000001</v>
+        <v>0.70840000000000003</v>
       </c>
       <c r="E4">
-        <v>1.0337000000000001</v>
+        <v>0.70840000000000003</v>
       </c>
       <c r="F4">
-        <v>1.0337000000000001</v>
+        <v>0.70840000000000003</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1566,13 +1542,13 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1.393</v>
+        <v>1.0677000000000001</v>
       </c>
       <c r="E5">
-        <v>1.393</v>
+        <v>1.0677000000000001</v>
       </c>
       <c r="F5">
-        <v>1.393</v>
+        <v>1.0677000000000001</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1604,13 +1580,13 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>1.0677000000000001</v>
+        <v>0.70840000000000003</v>
       </c>
       <c r="E6">
-        <v>1.0677000000000001</v>
+        <v>0.70840000000000003</v>
       </c>
       <c r="F6">
-        <v>1.0677000000000001</v>
+        <v>0.70840000000000003</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1718,13 +1694,13 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <v>0.91449999999999998</v>
+        <v>0.23</v>
       </c>
       <c r="E9">
-        <v>0.91449999999999998</v>
+        <v>0.23</v>
       </c>
       <c r="F9">
-        <v>0.91449999999999998</v>
+        <v>0.23</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1794,13 +1770,13 @@
         <v>6</v>
       </c>
       <c r="D11">
-        <v>0.55530000000000002</v>
+        <v>0.23</v>
       </c>
       <c r="E11">
-        <v>0.55530000000000002</v>
+        <v>0.23</v>
       </c>
       <c r="F11">
-        <v>0.55530000000000002</v>
+        <v>0.23</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1827,11 +1803,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9478548B-5118-4356-90D8-101DC853F820}">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F487C5B-ACDA-400B-BD13-B4C0C88E357C}">
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C15"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,7 +1822,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1864,22 +1840,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1917,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E4">
         <v>150</v>
@@ -1929,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1943,7 +1919,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E5">
         <v>150</v>
@@ -1955,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1969,7 +1945,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E6">
         <v>150</v>
@@ -1981,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1995,7 +1971,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E7">
         <v>150</v>
@@ -2007,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2015,13 +1991,13 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2033,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2041,13 +2017,13 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C9" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2059,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2067,13 +2043,13 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C10" s="13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2085,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2093,13 +2069,13 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2111,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2122,10 +2098,10 @@
         <v>43</v>
       </c>
       <c r="C12" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2137,85 +2113,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="13">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="13">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2224,11 +2122,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BE5B0D-6A2F-4A93-AC2C-50B71F113FCE}">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2CCBB1-2120-473B-B378-1400CF929E80}">
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C15"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,7 +2142,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2262,22 +2160,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2317,19 +2215,19 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2343,19 +2241,19 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2369,19 +2267,19 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2395,19 +2293,19 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2415,25 +2313,25 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2441,25 +2339,25 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C9" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2467,25 +2365,25 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C10" s="13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2493,25 +2391,25 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2522,100 +2420,22 @@
         <v>43</v>
       </c>
       <c r="C12" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="13">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="13">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2624,11 +2444,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2A7381-3CB4-48A5-96AD-E4A8217F5D90}">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EB492D-9017-47E9-A2F5-6B303F4E34DC}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C15"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2642,7 +2462,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2659,19 +2479,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2708,16 +2528,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2731,16 +2551,16 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2754,16 +2574,16 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2777,16 +2597,16 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2794,22 +2614,22 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2817,22 +2637,22 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C9" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2840,22 +2660,22 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C10" s="13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2863,22 +2683,22 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2889,88 +2709,19 @@
         <v>43</v>
       </c>
       <c r="C12" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="13">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="13">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2979,11 +2730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6870AD5D-AEF1-4457-9E7A-00B4863954B0}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68703E0-8626-4156-9DBA-ACB1A1B5A276}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C15"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2997,7 +2748,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3013,16 +2764,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3054,7 +2805,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E4">
         <v>500</v>
@@ -3071,7 +2822,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E5">
         <v>500</v>
@@ -3088,7 +2839,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E6">
         <v>500</v>
@@ -3105,7 +2856,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E7">
         <v>500</v>
@@ -3116,13 +2867,13 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -3133,13 +2884,13 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C9" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -3150,13 +2901,13 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C10" s="13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -3167,13 +2918,13 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -3187,63 +2938,12 @@
         <v>43</v>
       </c>
       <c r="C12" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="13">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="13">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15">
         <v>3</v>
       </c>
     </row>
@@ -3253,11 +2953,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FDB89A-9348-4228-AEF6-AF9930E7A2C6}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D12E12-F916-4216-A814-4ABD4843374B}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C15"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,7 +2971,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3287,16 +2987,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3330,13 +3030,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3350,13 +3050,13 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3370,13 +3070,13 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3390,13 +3090,13 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3404,19 +3104,19 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3424,19 +3124,19 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C9" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3444,19 +3144,19 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C10" s="13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3464,19 +3164,19 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3487,76 +3187,16 @@
         <v>43</v>
       </c>
       <c r="C12" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="13">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="13">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3565,11 +3205,11 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B843E9-DFE4-4AE3-B02B-084AA51A807F}">
-  <dimension ref="A1:I15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28453A40-BA6E-4807-8DD5-5C0CE181B824}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C15"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,7 +3226,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3605,25 +3245,25 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3664,16 +3304,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E4">
         <v>6000</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H4">
         <v>500</v>
@@ -3690,16 +3330,16 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E5">
         <v>5000</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H5">
         <v>500</v>
@@ -3716,16 +3356,16 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E6">
         <v>6000</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H6">
         <v>500</v>
@@ -3742,16 +3382,16 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E7">
         <v>5000</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H7">
         <v>500</v>
@@ -3762,22 +3402,22 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E8">
         <v>5000</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I8">
         <v>3</v>
@@ -3788,22 +3428,22 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C9" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E9">
         <v>5000</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I9">
         <v>3</v>
@@ -3814,22 +3454,22 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C10" s="13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E10">
         <v>5000</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I10">
         <v>3</v>
@@ -3840,22 +3480,22 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E11">
         <v>5000</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I11">
         <v>3</v>
@@ -3869,99 +3509,21 @@
         <v>43</v>
       </c>
       <c r="C12" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E12">
-        <v>7071.07</v>
+        <v>7810.25</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13">
-        <v>7071.07</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="13">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14">
-        <v>7810.25</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="13">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15">
-        <v>7810.25</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I15">
         <v>3</v>
       </c>
     </row>
@@ -3971,11 +3533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B150B06-4D33-48F5-BB4A-8FEAF4558352}">
-  <dimension ref="A1:F15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3476D7E1-19F9-4ED8-A9B9-D2B2D2FC5146}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C15"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3989,7 +3551,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4005,16 +3567,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4048,13 +3610,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4068,13 +3630,13 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4088,13 +3650,13 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4108,13 +3670,13 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4122,19 +3684,19 @@
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4142,19 +3704,19 @@
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C9" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4162,19 +3724,19 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C10" s="13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4182,19 +3744,19 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4205,76 +3767,16 @@
         <v>43</v>
       </c>
       <c r="C12" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="13">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="13">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4283,7 +3785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7146EA3-9722-4D3A-87DD-0D75BDEE2D63}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FA4DD0-40ED-4D5D-8B0A-5A92E560A509}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4309,7 +3811,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4329,52 +3831,52 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -4413,13 +3915,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D4">
         <v>300</v>
@@ -4452,10 +3954,10 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4464,7 +3966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0C103D-B759-4E28-BDC3-8DD0DC5CCEF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E975047-9446-41C9-A29E-9790834A4045}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4492,7 +3994,7 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4526,94 +4028,94 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB2" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>149</v>
-      </c>
       <c r="AC2" s="11" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="AD2" s="11" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -4630,40 +4132,40 @@
         <v>13</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>16</v>
@@ -4694,16 +4196,16 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E4">
         <v>11721.3</v>
@@ -4790,7 +4292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3506CFEF-254F-44A5-9A4A-B5EDCBEEFEFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F1C6E1-CA98-417F-87A0-BF89DDAAAAE7}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4808,7 +4310,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4818,19 +4320,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>22</v>
@@ -4858,22 +4360,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -4882,7 +4384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83221338-8DD4-4A4B-A77E-35179DC72205}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4350D4-66C1-43C3-9A88-1F5BA4643BF9}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4995,7 +4497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E391ABD-C050-4DD7-85ED-90F56AB50024}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9BC466-69C9-4C44-9A50-DB196A2188B4}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5011,7 +4513,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5030,7 +4532,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>4</v>
@@ -5091,22 +4593,22 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5120,22 +4622,22 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5149,22 +4651,22 @@
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -5178,22 +4680,22 @@
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -5202,7 +4704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590C13C5-2A7E-43A0-A875-42F37BE79724}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FCC78B-1A8C-4176-9D0A-AFF3D25773E6}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5219,7 +4721,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5234,13 +4736,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5271,7 +4773,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5285,7 +4787,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5299,7 +4801,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5313,7 +4815,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -5327,10 +4829,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -5344,10 +4846,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -5361,10 +4863,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -5378,10 +4880,10 @@
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -5390,7 +4892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5306E668-4674-48CE-88FC-2201D88114D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48ABF4B-CD5F-40E8-8EBF-0A2DE42E907B}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5409,7 +4911,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5432,34 +4934,34 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>22</v>
@@ -5479,22 +4981,22 @@
         <v>13</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>16</v>
@@ -5517,7 +5019,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E4">
         <v>5000</v>
@@ -5544,7 +5046,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -5558,7 +5060,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E5">
         <v>5000</v>
@@ -5585,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -5599,7 +5101,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E6">
         <v>5000</v>
@@ -5626,7 +5128,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -5640,7 +5142,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -5667,7 +5169,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -5676,7 +5178,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B1EA7F-86D3-4E0C-8E80-CBF2499622F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BD1E40-8BD7-4F76-A31A-39EFEDC92631}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5699,7 +5201,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5713,31 +5215,31 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>22</v>
@@ -5777,34 +5279,34 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -5813,7 +5315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A5C4F1-BA9A-4F35-B467-89BB4A6D10CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C60FF4A-C8D0-4146-B0D4-52A4B33A5EE9}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5832,7 +5334,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1"/>
@@ -5844,28 +5346,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5876,28 +5378,28 @@
         <v>13</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C4">
         <v>2.4000000000000001E-5</v>
@@ -5920,10 +5422,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C5">
         <v>7.7000000000000001E-5</v>
@@ -5940,10 +5442,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C6">
         <v>7.7000000000000001E-5</v>
@@ -5960,10 +5462,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C7">
         <v>7.7000000000000001E-5</v>
@@ -5990,7 +5492,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1E099B-E980-4271-8A62-F5596DD9857D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD111634-1AF7-4EC7-BF47-CCF0AB3FA698}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6005,13 +5507,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>22</v>
@@ -6027,10 +5529,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -6039,11 +5541,11 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F9E0A0-B189-4EFF-8ECB-01F3CCEFA662}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC28C7CA-2A79-4F7F-87E6-8B80C441323A}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A8"/>
+      <selection activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6056,7 +5558,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1"/>
@@ -6069,7 +5571,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>10</v>
@@ -6078,7 +5580,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>22</v>
@@ -6109,7 +5611,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -6121,7 +5623,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6129,7 +5631,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>6000</v>
@@ -6141,7 +5643,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6149,7 +5651,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>6000</v>
@@ -6161,7 +5663,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -6169,7 +5671,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -6181,7 +5683,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -6190,11 +5692,11 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674515EC-FABD-44DF-9E7E-401FD958ACDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B34DB6-03BA-40F5-A4CF-B475FC9C3A7C}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D11"/>
+      <selection activeCell="D4" sqref="A4:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6209,7 +5711,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6222,19 +5724,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -6283,7 +5785,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
@@ -6292,7 +5794,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -6304,7 +5806,7 @@
         <v>5000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6312,7 +5814,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
@@ -6321,7 +5823,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F5">
         <v>6000</v>
@@ -6333,7 +5835,7 @@
         <v>5000</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6341,7 +5843,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
@@ -6350,7 +5852,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F6">
         <v>6000</v>
@@ -6362,7 +5864,7 @@
         <v>5000</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6370,7 +5872,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>17</v>
@@ -6379,7 +5881,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -6391,7 +5893,7 @@
         <v>5000</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6399,7 +5901,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>18</v>
@@ -6408,7 +5910,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -6420,7 +5922,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -6428,7 +5930,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
@@ -6437,7 +5939,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F9">
         <v>6000</v>
@@ -6449,7 +5951,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -6457,7 +5959,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>18</v>
@@ -6466,7 +5968,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F10">
         <v>6000</v>
@@ -6478,7 +5980,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -6486,7 +5988,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>18</v>
@@ -6495,7 +5997,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -6507,7 +6009,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -6516,7 +6018,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D6A5AB-B42B-42EF-B904-9016BE2983FF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA831AC8-0F87-4432-B91D-CCAD69B797A4}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6532,17 +6034,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -6561,13 +6063,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -6576,7 +6078,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2863531-406A-430E-87BD-D1A88C822BCB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E671C232-1BBC-4E88-AA20-2AE7D34880BC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6596,7 +6098,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="4"/>
@@ -6607,22 +6109,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>22</v>
@@ -6659,19 +6161,19 @@
         <v>5000</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -6680,7 +6182,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3B6526-088B-4E1B-BB31-CC71C20E6CFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995347AA-CF1B-4032-9FCD-FB149DA08E59}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6853,7 +6355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8C7A18-925F-4EB6-9D23-680231FB1C42}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F6C2E6-18A4-4779-B57C-A7D11CE73B54}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6872,7 +6374,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6883,25 +6385,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6929,13 +6431,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
@@ -6944,7 +6446,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -6953,7 +6455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232BD04B-EAE9-48EC-80A3-7030A9BE29D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFEDCF4-B33A-4025-92A5-843E6043F546}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -6978,7 +6480,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6994,40 +6496,40 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="K2" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="L2" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -7070,40 +6572,40 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -7112,11 +6614,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60F2443-A839-473C-8EC1-2308F09D0501}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C20E1-A343-4444-9BC0-D54BCF2141FE}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C7"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7125,7 +6627,7 @@
     <col min="2" max="2" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -7176,67 +6678,16 @@
         <v>43</v>
       </c>
       <c r="B4" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="13">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="13">
-        <v>3</v>
-      </c>
-      <c r="C6" s="13">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="13">
-        <v>2</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -7245,11 +6696,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AE323D-8169-4A3A-B5B6-B72036F5584B}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809BE8B6-D733-448F-B6AD-19555F05ACCE}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E7"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7260,12 +6711,12 @@
     <col min="4" max="4" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7282,7 +6733,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>34</v>
@@ -7322,7 +6773,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
@@ -7331,85 +6782,16 @@
         <v>43</v>
       </c>
       <c r="D4" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>7071.07</v>
+        <v>7810.25</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="13">
-        <v>6</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>7071.07</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D6" s="13">
-        <v>4</v>
-      </c>
-      <c r="E6" s="13">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>7810.25</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="13">
-        <v>2</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>7810.25</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -7418,7 +6800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E58660-77AF-4DEB-AC51-8EB56E7E1162}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561569BA-DB1C-48E8-88C1-1C9B0683A820}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7436,7 +6818,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7479,7 +6861,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B4" s="13">
         <v>2</v>
@@ -7491,12 +6873,12 @@
         <v>44</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
@@ -7508,12 +6890,12 @@
         <v>44</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B6" s="13">
         <v>4</v>
@@ -7525,12 +6907,12 @@
         <v>44</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B7" s="13">
         <v>3</v>
@@ -7542,7 +6924,7 @@
         <v>44</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -7551,7 +6933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2541EC49-4831-4E5C-B5F1-7E31C4D084CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDCC2BB-F032-4011-857A-6E938C695689}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7571,7 +6953,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7588,7 +6970,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>34</v>
@@ -7634,7 +7016,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D4" s="13">
         <v>2</v>
@@ -7646,18 +7028,18 @@
         <v>5000</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D5" s="13">
         <v>5</v>
@@ -7669,18 +7051,18 @@
         <v>5000</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D6" s="13">
         <v>6</v>
@@ -7692,18 +7074,18 @@
         <v>5000</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D7" s="13">
         <v>4</v>
@@ -7715,7 +7097,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -7724,7 +7106,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F8903F-5C46-461B-9208-57025B7FD9B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE7EC35-43B0-40DE-9996-6997DC56B8F1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7740,17 +7122,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -7769,13 +7151,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -7784,7 +7166,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C0B1E2-CF61-4D62-BF2B-E389D0E6B00F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBDE068-3256-4E03-852E-1FE5F056C80F}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7803,7 +7185,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1"/>
@@ -7819,34 +7201,34 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>36</v>
@@ -7895,10 +7277,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -7928,7 +7310,7 @@
         <v>6000</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>